<commit_message>
Working version of Oneto-Denier flow model
Add major boundary conditions to match historical hydrographs
Start preparing plotting output for work
Minor adjustments to other projects to improve coding practices
</commit_message>
<xml_diff>
--- a/Projects/Streambed_seepage/model_documentation.xlsx
+++ b/Projects/Streambed_seepage/model_documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrewc\Documents\GitHub\CosumnesRiverRecharge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajcalder\Documents\GitHub\CosumnesRiverRecharge\Projects\Streambed_seepage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E34CD08-E560-4CC1-82BE-A4C32BD5599D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6565426C-0059-40B1-826B-F91F7FD6AD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Geology" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>Subject</t>
   </si>
@@ -52,6 +53,115 @@
   </si>
   <si>
     <t>Break up notes by model packages (e.g., SFR) and major updates (e.g., model extension) or areas of focus (e.g., vineyards)</t>
+  </si>
+  <si>
+    <t>tried removing reduction of 1/10 to sfr vka to see if that increases signal in GW response</t>
+  </si>
+  <si>
+    <t>I'm curious why the lak package requires basic package to be negative, this messes with MW23 which is screened in layer 1. I updated the screened depth for MW23, Oneto-Ag and now they are below layer 1 so no issue</t>
+  </si>
+  <si>
+    <t>after adding the lake to the simulation, the run time is still only 14 min long, although issue in SS with high GWE due to lake steady state,</t>
+  </si>
+  <si>
+    <t>11 min run time after making SS for lake dry</t>
+  </si>
+  <si>
+    <t>Fixed SFR layer, removed EVT where there were SFR cells. run time was 17 min after removing EVT under sfr cells and fixing sfr layer</t>
+  </si>
+  <si>
+    <t>changing the sfr layer really impacted the VKA for SFR because I had defaulted the layer to 0, but changing the dem meant the str top was lower than it was so there was likely a conflict between the UPW VKA and SFR VKA.</t>
+  </si>
+  <si>
+    <t>original Oneto-Denier dem, max sim GWL around 3-4 m. raising the str top by 4 m brought max sim gwl to 6-8 m and the sim values were raised so the mean level was higher to the peaks seen in the obs, but is to far above the dry season lows. There isn't a large peak still so the peak is likely due to over bank flooding</t>
+  </si>
+  <si>
+    <t>adding 4m to the str top had run time of 48 min</t>
+  </si>
+  <si>
+    <t>the smaller peak flows might also be a result of the cross-section change resulting in different depths/widths or even different stream bottom elevations</t>
+  </si>
+  <si>
+    <t>adding the missing sfr segments brought up the steady state levels so that even with ET the model matches with observed, now the peaks of gwl are well above the simulation which is likely because we aren't simulating the flooding or precipitation from winter events</t>
+  </si>
+  <si>
+    <t>Adding the extra stream segments could have increased conflict with EVT? run time was 37 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The HEC-RAS dem only extended to the upper end of Oneto-Denier, so the original model runs which ran in 3min actually only had SFR for the first 1/3-1/2 of the domain. I ran the XS code again for the 1m dem from Alison Whipple but now the code runs slow and has issues. It doesn't seem like it's the VKA because the first few segments have the highest conductivity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With the outflow the head within the basin is largely controlled by the GHB head (ranges 5-15m, gw head below river defaults to 10m) which is not desirable. I need better justification for the outflow choices. Parsimony dicatates less is more. </t>
+  </si>
+  <si>
+    <t>Initial set up was a year long flow test with the primary boundary condition the SFR package and the GHB included to allow lateral groundwater outflow which is expected as the water entering the perched aquifers may transfer horizontally. Added evapotranspiration with EVT to allow dry season perched aquifer usage. Recharge was added then removed because it caused too much of a jump in levels. Added lake package to represent floodplain recharge in the 2D floodplain.</t>
+  </si>
+  <si>
+    <t>Initial set up</t>
+  </si>
+  <si>
+    <t>SFR</t>
+  </si>
+  <si>
+    <t>Packages</t>
+  </si>
+  <si>
+    <t>XS delination</t>
+  </si>
+  <si>
+    <t>Channel elevation</t>
+  </si>
+  <si>
+    <t>SFR layer</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>Lake</t>
+  </si>
+  <si>
+    <t>DEM</t>
+  </si>
+  <si>
+    <t>The monitoring well ground elevations sampled from the 2m DEM (from Lily Tomkovic) are within ~0.5m of the elevations found with the regional 10m DEM so it is unlikely a data issue at the well heads for the observation data.
+There is a 2-8m discrepancy between the regional 10m and local 2m DEM when we look at the stream top. And this impacts how much seepage we have from the stream to the adjacent cells.
+The cause was when writing out the XS data, I had forgot to adjust for the conversion or lack thereof from ft to meters that was put in previously for the HEC-RAS dem. Stream top now shows expected range of 5-2m rather than 2-0.5.</t>
+  </si>
+  <si>
+    <t>SFR-DEM</t>
+  </si>
+  <si>
+    <t>It is important to note an update in shapely caused a change in code. The NHD line string must be inserted into linemerge() after applying a unary_union. And the linemerge function is critical as it joins the line strings based on the closest end points which is key to properly sorting the line into a good direction.</t>
+  </si>
+  <si>
+    <t>After fixing the DEM issue in the SFR package, runtime reduced to 8 min. And now simulated peaks are upt to 7 m but the baseline gwl levels are higher as expected because the stream level is higher. This could mean that ET could be higher or maybe deeper?</t>
+  </si>
+  <si>
+    <t>The water levels are undersimulated in the lake which is because right now the lake is only acting as an outflow of groundwater, it isn't causing recharge. Need to see if there isn't flow entering the lake. Or if lake minimum is too low?</t>
+  </si>
+  <si>
+    <t>DIS</t>
+  </si>
+  <si>
+    <t>Deepened model thickness from 20m to 40m to allow inclusion of agricultural pumping in deeper layers to draw down head during the summer and also improve characterization of Oneto-Ag which is screened deeper (avoids boundary effects on other wells too). Adding the extra layers seems to have buffered the effects of groundwater change due to stream flow - &gt; messed up lake package.</t>
+  </si>
+  <si>
+    <t>Added average evapotranspiration rate to lake because I believe ET is removed with no flow cells.
+The issue might be that if the lake stage starts below the minimum then modflow can't bring it back to saturation even with inflow.
+I updated the THETA NSSITR SSCNR SURF parameters to use shasta's -1 &gt; 1, 0 &gt; 1000, 0.01 &gt; 1E-5 and 0 &gt; 0.02 (1 1000 1E-5 0.02) which then made the lake have stage changes. Now the lake stage gets way to high because there is a lot of inflow and the only outflow is seepage and ET, need to add the surface water outflow. (Runtime jumped to 27 minutes)
+Adding lake outflow brought runtime back to 7 min.</t>
+  </si>
+  <si>
+    <t>WEL</t>
+  </si>
+  <si>
+    <t>Adding pumping for the agricultural production in the area caused a drawdown of 15 m in the following season which is 10 m + more than needed.
+ After removing pumping where there are GDE's identified (a reduction of 1/3-1/2 for the SS), the dry season decline was only 5 m too much, it might also be that I'm still simulating a confined system when this should be a semi-confined system. The pumping for the summer should be 0.6-1m of water which for Sy of 0.25 is 2.4-4m decline but 0.1 would be 6-10m. In confined terms we have Ss*b of 0.001 to 0.004 which would be even more. Let's run a test of the system unconfined (previous run times were 9m on avg)</t>
+  </si>
+  <si>
+    <t>Adding the unconfined, OWHM through an error finally saying the streambed bottom elevations were below cell bottoms, maybe in confined conditions it asssumes this is a non-issue. I found the issue and corrected the SFR layer but OWHM kept raising an error until I added the option FIX_STREAM_BOTTOM (30 min)
+The monitoring well dynamics look pretty good after adjusting the top 5 layers as unconfined, now pumping doesn't draw them down too much and we still see proper rise. The only other adjustment would be to set a higher threshold for floodplain inundation because some wells seem to have to much recharge in smaller, earlier events</t>
   </si>
 </sst>
 </file>
@@ -383,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,6 +506,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -403,14 +518,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127FF96A-09F0-493D-9D8B-9F102DA87FD1}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="94.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -428,12 +544,230 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+    <row r="2" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>44955</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>44955</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>44953</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>44953</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>44952</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>44952</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>44951</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>44949</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>44949</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>44949</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>44949</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>44949</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -445,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38AFD942-8E80-472F-A04D-2043AB373721}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updates to fix convergence issue
</commit_message>
<xml_diff>
--- a/Projects/Streambed_seepage/model_documentation.xlsx
+++ b/Projects/Streambed_seepage/model_documentation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajcalder\Documents\GitHub\CosumnesRiverRecharge\Projects\Streambed_seepage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6565426C-0059-40B1-826B-F91F7FD6AD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E149D6C4-BAF5-479D-A29A-5E57D10A6660}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,6 @@
     <sheet name="Geology" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
   <si>
     <t>Subject</t>
   </si>
@@ -162,6 +161,61 @@
   <si>
     <t>Adding the unconfined, OWHM through an error finally saying the streambed bottom elevations were below cell bottoms, maybe in confined conditions it asssumes this is a non-issue. I found the issue and corrected the SFR layer but OWHM kept raising an error until I added the option FIX_STREAM_BOTTOM (30 min)
 The monitoring well dynamics look pretty good after adjusting the top 5 layers as unconfined, now pumping doesn't draw them down too much and we still see proper rise. The only other adjustment would be to set a higher threshold for floodplain inundation because some wells seem to have to much recharge in smaller, earlier events</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Homogeneous</t>
+  </si>
+  <si>
+    <t>I set up a homogeneous model run that averages all values to one for hk, vka. HK is sandy mud, vka is mud. Issue is that the cumulative mass error was still 9% so it may be that the clogging layers are not the issue?</t>
+  </si>
+  <si>
+    <t>Finally realized that the mass budget error is very large during the peak flow event leading to an unacceptable cumulative mass error. Increasing the maxouter from 500 to 1000 didn't make a difference beside runtime. I'm going to scale back lake bed and sfr vka by 1/10 again as realistically they should be clogged at least in the sand and gravel. The error actually increased to 14%</t>
+  </si>
+  <si>
+    <t>Cumulative error is still hitting 11% after adjustments because in spd 50 the error hits 38% and doesn't return to near 0 after that. I need to assess if the lake is the cause of these issues by removing it. It might also take tighter convergence criteria because the model is solving each stress period quick so it isn't being required to converge sufficiently. Without the lake package the model hits an error of 16% at spd 50 then returns to near 0% error within 2 stress periods. 
+For the Blodgett Dam project I used a theta value of -0.75. The error propagation was the same with 0.75
+I used 0.5 for the lake water budget for the setback_streamflow run, this had the same results as before. There must be a need for convergence criteria then.</t>
+  </si>
+  <si>
+    <t>Setting NWT flow tolerance from 500 to 15 didn't improve. Need to reassess if there is a descrepancy in the set up of the lake package. I removed LAK grid cells that had less than 50% coverage of a cell also because there is likely some overlap with SFR grid cells. Max error started at 16% then quickly went to near 0 within several stress periods. Cumulative volumetric error is 3.84%</t>
+  </si>
+  <si>
+    <t>The lake bathymetry set up I had been using was converting the units from ft to meters when it was already in meters so lake volume was essenentialy 1/10 what it should be per stage. Didn't make a noticeable difference. It actually did make a difference I had coded the lakarr correction wrong where I only used cells over the stream, fixed that so now there are no cells over streams and error CME was 0.12%. Runtime 16 min</t>
+  </si>
+  <si>
+    <t>I re ran the parallel runs but I didn't include the upate for maxiter from 500 to 100 or fluxtol from 500 to 15. But those didn't make a big difference anyway</t>
+  </si>
+  <si>
+    <t>Parallel</t>
+  </si>
+  <si>
+    <t>Model fit</t>
+  </si>
+  <si>
+    <t>Running with udpated work from complex model only takes 10 min (0.1% error)</t>
+  </si>
+  <si>
+    <t>Playing around with the model set up to improve water budget error reduced the NSE and increased RMSE slightly. Not sure if this is because of the reduced sfr/lake vka or just because of reducing the number of cells.
+I noticed Oneto-Ag wasn't included in hobout because of naming convention issues.
+The issue with not enough dry season drawdown again is odd because I'm not sure what could have impacted it. The solution would be to reduce the number of unconfined layers to cause more head fluctuation with storage change or to increase horizontal conductivity to increase drainage rates.
+What's tricky is that some of the worst performing realizations have too much drawdown so it's not something I should really play with. I could adjust it to match for the steady state and then leave as is?</t>
+  </si>
+  <si>
+    <t>Comparing the R2, RMSE, NSE from the parallel set up with flow error of 500 m3/d and maxouter of 500 to the test model with 15 m3/d and 500 maxouter showed slightly worse values so tighter convergence criteria help with matching reality as well (probably avoids extreme stage values). When considering model error 500 m3/day is 1/5 of a cfs so 500 is really sufficient.</t>
+  </si>
+  <si>
+    <t>The hydrographs between the homogeneous and one heterogeneous are not so different.
+The groundwater contours showed the most noticeable difference, in the homogeneous case they were much more uniform and no pumping depression formed on the eastern boundary.
+Checking the packages showed the SFR/LAK package hadn't been written with uniform VKA properly, instead variable from tprogs</t>
+  </si>
+  <si>
+    <t>Boundary Conditions</t>
+  </si>
+  <si>
+    <t>The model is showing a larger than realistic pumping depression below the field site which means either too much pumping or not enough inflow from the delta</t>
   </si>
 </sst>
 </file>
@@ -518,15 +572,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127FF96A-09F0-493D-9D8B-9F102DA87FD1}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="94.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -544,228 +599,349 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>44955</v>
-      </c>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>44955</v>
+        <v>44964</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>44953</v>
+        <v>44964</v>
       </c>
       <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>44964</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>44963</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>44963</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>44953</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>44952</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>44952</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>44951</v>
+        <v>44963</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>44949</v>
+        <v>44963</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>7</v>
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>44949</v>
+        <v>44959</v>
       </c>
       <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>44959</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>44958</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>44955</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>44955</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>44953</v>
+      </c>
+      <c r="B16" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>44949</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>44953</v>
+      </c>
+      <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>44949</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>44949</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>44952</v>
+      </c>
+      <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>44944</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>44944</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>44944</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>44944</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>44944</v>
+        <v>44952</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>44944</v>
+        <v>44951</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>44944</v>
+        <v>44949</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>44949</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>44949</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>44949</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>44949</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+    <row r="33" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
         <v>44944</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B33" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -975,7 +1151,7 @@
       <c r="A25" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D26">
+  <sortState ref="A2:D26">
     <sortCondition descending="1" ref="A2:A26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>